<commit_message>
Fix(nominas): Corrige errores en edición y borrado de nóminas
Se soluciona un error que impedía editar y borrar nóminas persistentes debido a una falta de coincidencia de parámetros entre el frontend y el backend.

Se ajusta la estructura de datos devuelta por el API para la edición de nóminas, asegurando que el formulario se llene correctamente.
</commit_message>
<xml_diff>
--- a/excepciones.xlsx
+++ b/excepciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,25 +463,106 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>35115887</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Analia Belen Miño</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CASA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Roberto Laforcada</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>53412356</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Paris Laforcada</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CASA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Roberto Laforcada</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>35115812</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lisandro Laforcada</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Roberto Laforcada</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>59610581</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Patrick Laforcada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Roberto Laforcada</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>2025-11-09</t>
         </is>

</xml_diff>

<commit_message>
Salvado con todas las modificaciones funcionales, antes de ejecutar la compilacion
</commit_message>
<xml_diff>
--- a/excepciones.xlsx
+++ b/excepciones.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,48 +463,54 @@
           <t>Fecha de Alta</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vigencia</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>35115887</t>
+          <t>33013638</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Analia Belen Miño</t>
+          <t>Roberto  Laforcada</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CASA</t>
+          <t>IRSA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Roberto Laforcada</t>
+          <t>Maximiliano Godoy</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
-        </is>
-      </c>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>53412356</t>
+          <t>35115887</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Paris Laforcada</t>
+          <t>Analia Belen Miño</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Casa</t>
+          <t>IRSA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -510,24 +520,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
-        </is>
-      </c>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>35115812</t>
+          <t>53412356</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lisandro Laforcada</t>
+          <t>Paris Laforcada</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Casa</t>
+          <t>IRSA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,9 +548,10 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
-        </is>
-      </c>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -554,7 +566,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Casa</t>
+          <t>IRSA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,8 +576,11 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
-        </is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>46003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>